<commit_message>
Add Progess Bar to GUI
</commit_message>
<xml_diff>
--- a/WebScrapedItems.xlsx
+++ b/WebScrapedItems.xlsx
@@ -501,16 +501,8 @@
           <t>GPFCE-WNDSCRN</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/wind-screen-round-transparent-800px.png</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Enjoying the great outdoors doesn't have to stop just because it's a little windy. Add the Round Windscreen to your Hamptons Patioflame® Table and keep the fun going even if there's a breeze. The five inch tall tempered glass offers protection so that the flames don't get blown out.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -531,16 +523,8 @@
           <t>55015</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/55015-Locking-tongs-800px-1.png</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Grill enthusiasts around the globe say that the most important tool in their arsenal is a good set of tongs. And Napoleon's Stainless Steel Tongs are the best ones for the job. Starting with the perfect length, these tongs are not too short, nor too long. The rubberized grip inserts keep the tongs cool to the touch and give extra gripping power when in use. The 16-inches of stainless steel feel balanced and are easy to use in dainty hands or big strong ones. These Stainless Steel Tongs feature a sensitive spring action that allows them to be incredibly dexterous. Pick up a single pea with these tongs, or flip something larger than a two-pound steak. The scalloped ends grip food nicely without piercing the food and spilling the juices. Lock these tongs closed for easy storage. They fit in the kitchen drawer easily. Or hang them from the convenient loop.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -583,16 +567,8 @@
           <t>61010</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/61010-digital-thermometer-800px.png</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Relax while cooking all your meats on the grill. The Fast Read Digital Thermometer will let you know when the meat is done. Without cutting into meat and potentially losing all of those precious juices, simply push the steel rod into the center of your meat or fish, the LED display will show the temperature within 4 to 5 seconds in either Celsius or Fahrenheit. Clean the stem with soap and water only, do not wash in the dishwasher. The best way to know if your food is cooked to safe standards and perfectly done to your liking is to use an accurate digital thermometer. Napoleon's Fast Read Digital Thermometer is ideal for use on the barbecue grill, oven and even the frying pan. Instantly know whether your meal is cooked to perfection without leaving it up to chance. Clever, multifunctional and easy to maintain, every kitchen benefits from the addition of a Napoleon barbecue accessory. Our accessories provide you with the essentials to create delicious grilled food and then some to enhance your cooking arsenal with a wide variety of creative additions to broaden your culinary horizons.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -613,16 +589,8 @@
           <t>62007</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/62007-grease-trays-transparent-800px.png</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Protect your grill and make it easier to clean by using these disposable aluminum Drip Trays in your barbecue grill. Used to collect grease and debris that may not be burned off while grilling, these trays go in the bottom of the grill at the back. As part of your regular grill maintenance, these trays should be checked and changed every four to six cooking sessions, depending on how much barbecuing you do. Dump any leavings from these Drip Trays and easily recycle for fast and simple barbecue grill maintenance. Use these on the barbecue for side dishes and food storage if preparing grilled goodies for a potluck as well. Just remember to give them a rinse and clean before use. Keep your Napoleon Grill clean and make maintenance easier by using a disposable drip tray today. Clever, multifunctional and easy to maintain, every kitchen benefits from the addition of a Napoleon barbecue accessory. Our accessories provide you with the essentials to create delicious grilled food and then some to enhance your cooking arsenal with a wide variety of creative additions to broaden your culinary horizons.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -643,16 +611,8 @@
           <t>62056</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/62056-SS-CleaningBrushwScraper-transparent-800px.png</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Use the Napoleon Brass Bristle Wide Grill Brush to keep your Porcelain Enameled Cast Iron Cooking Grids clean. A clean grill is a happy grill. You should brush the stuck-on foods from your barbecue with a grill brush after every time you grill, while the grill is still hot, and again before grilling your next meal. The brass bristles on the Brass Bristle Wide Grill Brush will not damage your Porcelain Enameled Cast Iron Cooking Grids but will last a long time. The Brass Bristle Wide Grill Brush is eighteen inches long with a heat-safe grip on its ergonomic handle, giving you easy leverage for getting at that tough stuck-on food. This barbecue grill brush has a metal scraper on the head for particularly tough spots. The Brass Bristle Wide Grill Brush features a hanger for easy storage which means your grill brush is always within reach. Clever, multifunctional and easy to maintain, every kitchen benefits from the addition of a Napoleon barbecue accessory. Our accessories provide you with the essentials to create delicious grilled food and then some to enhance your cooking arsenal with a wide variety of creative additions to broaden your culinary horizons.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -673,16 +633,8 @@
           <t>62050</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/62050-JETFIRE-Burner-Brush-800px.png</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;It's easy to keep your Napoleon Grill working efficiently and starting reliably by performing regular maintenance, which includes cleaning the JETFIRE™ Ignition and burner ports by using this maintenance kit. Use the brush to clean the electrode tip, and inside the pilot bracket on the JETFIRE™ Ignition. The drill bit is for clearing clogged burner ports on our stainless steel burners. Gently, using a small cordless drill, use this tool to remove any debris blocking ports, being careful not to flex the bit.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -703,16 +655,8 @@
           <t>62062</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/62062-Parallel-Brass-GrillBrush-800px.png</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;This Triple-Row Grill Brush with Brass Bristles is ideal for removing stuck-on residue from cast-iron cooking grids after grilling delicious barbecued meals. The curved handle design provides added leverage while cleaning. The vertical orientation of brush rows goes in between grids to provide an easier and better clean The convenient hook means this grill brush is always within reach.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -733,16 +677,8 @@
           <t>68002</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/68002-Large-grill-mat-800px.png</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Protect what's under your barbecue grill and show your Napoleon pride with the Napoleon Grill Mat For Large Grills. Great for ensuring your deck and patio are safe from oil and grease damage, this easy-to-clean mat is ideal for larger gas barbecue grills and measures 90 by 35-inches (228.6cm by 88.9 cm). If you're using a charcoal barbecue grill, this fire-resistant mat is perfect for providing protection against accidentally dropped coals and errant sparks. The non-slip, diamond plate pattern is a stylish grey color, ideal for upping your grill's flare factor while protecting your beautiful outdoor living area. This product is not recommended for use on composite decking. Clever, multifunctional and easy to maintain, every kitchen benefits from the addition of a Napoleon barbecue accessory. Our accessories provide you with the essentials to create delicious grilled food and then some to enhance your cooking arsenal with a wide variety of creative additions to broaden your culinary horizons.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -763,16 +699,8 @@
           <t>69911</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/6991X-Rostisserie-Kit-Rogue-Rotisserie-on-white-800px.png</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Whether you have a compact Rogue® 365, 425 or a large Rogue® 525 Series Model, this Stainless Steel, Heavy Duty, Multi-Piece Rotisserie Kit will fit your needs. Made with food grade stainless steel, the square spit rod features rod extensions to ensure that you can go the distance. The heavy-duty motor can turn up to 12 kilograms of a balanced load. The two four pronged forks will securely hold everything you could wish to spit roast and they tighten securely with easy to use thumb screws.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -793,16 +721,8 @@
           <t>70000</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/70000-on-white-personal-pizza-stones-800px.png</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Grill perfect personal pizzas for two with the Napoleon 10-Inch Personal Size Pizza / Baking Stone Set. There's nothing like fresh, homemade pizza, even when on the go. You can fit both pizza stones onto the grill, even on a TravelQ™. The porous stone pulls moisture away from your pizza crust and yields crispy and light results, just like pizza fresh from a pizzeria. Like your favorite cast iron frying pan, this stone will season over time, making it more effective. It is recommended that you hand wash your PRO Series Pizza Stone by hand, with warm water, once completely cooled. Avoid soapy water and scrubbing. Pair your Pizza Stone with the Napoleon Pizza Peel for added convenience.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -823,16 +743,8 @@
           <t>70007</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/70007-PRO-Replacement-Grill-Brush-Head-transparent-800px.png</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;No need to replace your entire PRO Series Stainless Steel grill brush, just use Napoleon replacement Brush Head. Comes with a bonus PRO series abrasive scrubber, perfect for getting to those well grilled on bits.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -919,16 +831,8 @@
           <t>90002</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/90002-PizzaStarterKit-all-transparent-800px.png</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Napoleon has a pizza party in a box for those who live for delicious homemade pizza. The Pizza Lover's Starter Kit has everything you need for a backyard pizza party except for the dough and toppings. Grill up the perfect medium-sized pizza on the Pizza Stone. The porous stone draws moisture away from the pizza dough for the perfect, crisp crust. Easily transfer your dough to the grill and then to your waiting friends and family with the Stainless Steel Pizza Peel, which folds for space saving storage. Cut the perfect slice with the included Pizza Wheel, and top everything off with a little extra cheese from the 2-in-1 Cheese Grater Slicer. If pizza is your passion, then this Pizza Lover's Starter Kit is perfect for you.  Clever, multifunctional and easy to maintain, every kitchen benefits from the addition of a Napoleon barbecue accessory. Our accessories provide you with the essentials to create delicious grilled food and then some to enhance your cooking arsenal with a wide variety of creative additions to broaden your culinary horizons.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -971,11 +875,7 @@
           <t>IM-UGC665-CN</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/IM-UGC665-UnderGrillBasket-Straight-Logo-800px.png</t>
-        </is>
-      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -997,11 +897,7 @@
           <t>IM-WSF-CN</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/IM-WSF-WallSpacer-800px-rev.png</t>
-        </is>
-      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -1023,11 +919,7 @@
           <t>BI-1824-2DR</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/BI-1824-2DR-Ang-Closed-800px.png</t>
-        </is>
-      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
@@ -1049,11 +941,7 @@
           <t>BI-3024-2D</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/BI-3024-2D-Ang-Closed-800px.png</t>
-        </is>
-      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
@@ -1075,16 +963,8 @@
           <t>61287</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/TravelQ-61287-PRO285X-cart-F-800px.png</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Protect your TravelQ™ PRO285 on Stand (PRO285-STAND) with this Premium Grill Cover. The durable, water-resistant fabric won't crack, and the improved UV inhibitors provide superior fade resistance. For year round, full weather protection for your grill, the Premium Grill Cover can't be beat. Adjustable straps with buckles keep the cover in place, while the vent allows for airflow preventing mildew, as well as protection on gusty days. Easily store your cover out of the way with the convenient hanging loops. The cover only fits with the side selves removed from the stand.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1105,16 +985,8 @@
           <t>61852</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Hamptons-Square-61852-Straight-800px.png</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Protect your Hamptons or Victorian Square Patioflame® Table with this Premium Square Patioflame® Table Cover. The durable, water-resistant fabric won't crack, and the improved UV inhibitors provide superior fade resistance. For year round, full weather protection for your Patioflame® Table the Premium Patioflame® cover can't be beat. The vent allows for airflow preventing mildew, as well as protection on gusty days. Easily store your cover out of the way with the convenient hanging loops. Use the Velcro panel on the front for easy access to the propane storage, and for easy covering and uncovering of your Patioflame® too. Use this Premium Patioflame® Table cover to protect other flame tables too. Refer to the on-package sizing description to find the right cover for you.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1135,16 +1007,8 @@
           <t>61286</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/TravelQ-61286-TQ285-F-800px.png</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Protect your favorite portable grill, the TravelQ™, with this durable, water resistant Premium Grill Cover for TravelQ™ 285 and PRO285. The fabric won't crack, and the improved UV inhibitors provide superior fade resistance. For year round full weather protection for your grill, the Premium Grill Cover can't be beat and is covered by a 3 year limited warranty.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1165,16 +1029,8 @@
           <t>61855</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Kensington-Round-61855-Cover-800px.png</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Protect your Kensington Round Patioflame® Table with this Premium Round Patioflame® Table Cover. The durable, water-resistant fabric won't crack, and the improved UV inhibitors provide superior fade resistance. For year round, full weather protection for your Patioflame® Table the Premium Patioflame® cover can't be beat. Adjustable straps with buckles secure the cover, while the vent allows for airflow preventing mildew, as well as protection on gusty days. Easily store your cover out of the way with the convenient hanging loops. Use the Velcro panel on the front for easy access to the propane storage, and for easy covering and uncovering of your Patioflame® Table too. Use this Premium Patioflame® Table cover to protect other flame tables too. Refer to the on-package sizing description to find the right cover for you.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1195,16 +1051,8 @@
           <t>61856</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Uptown-61856-Rectangle-Straight-800px.png</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Protect your Uptown PatioflameTable with this Premium Grill Cover. Durable, water-resistant fabric won't crack and UV inhibitors provide superior fade resistance. Adjustable straps with buckles keep the cover in place, while the vent allows for airflow preventing mildew, as well as protection on gusty days. Easily store your cover out of the way with the convenient hanging loops.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1247,16 +1095,8 @@
           <t>67002</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/maple-wood-chips-bag-transparent-800px.png</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;This hardwood is from the sugar maple tree and is also known as hard maple. Smoking with Maple Wood Chips is much like smoking with other fruitwoods like cherry. It gives the food being smoked a sweet and subtle, balanced flavor that is excellent, especially for ham and bacon. Maple Wood Chips are also great for poultry, pork, salmon, arctic char and trout. To use the Maple Wood Chips, soak them in water for at least 30 minutes before you are ready to smoke. They can also be soaked in apple juice, chardonnay, cabernet sauvignon, honey brown lager and maple lager for added flavor. When they have been sufficiently soaked, remove the Maple Wood Chips from the liquid and place them into a Napoleon Smoker Pipe, and place that pipe directly on the sear plates of your gas grill. Alternatively you can place soaked chips into the integrated smoker tray on the Prestige PRO™ Series PRO665RSIB Gas Grill, or directly onto the lit charcoal of an Apollo® 3 in 1 Charcoal Grill and Water Smoker. When the Maple Wood Chips begin to smoke, place the food on the grill and close the lid. Remember to keep the lid closed for the best smoked flavor.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1277,16 +1117,8 @@
           <t>67003</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/hickory-wood-chips-transparent-800px.png</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;The leafy Hickory tree is a species found abundantly around the world. It is a hardwood and is fantastic for long smoking meats, especially pork and bacon. The bold flavor produced by smoke from Hickory Wood Chips is bold and often associated with southern barbecue. Soak the Hickory Wood Chips in water for at least 30 minutes before you are ready to smoke. You don't have to use just water. Other liquid pairings go well with Hickory like beer, bourbon, ginger ale, Coke, apple juice, pineapple juice and even a cabernet sauvignon. Remove the wood chips from the liquid and place them in the Napoleon Smoker Tube, then directly onto the sear plates of your gas grill, on your burning charcoal in the Apollo® 3 in 1 Charcoal Grill and Water Smoker, or into the integrated Smoker Tray in the Napoleon Prestige PRO Series PRO665 Gas Grill. Once the Hickory Wood Chips begin to smoke, put the food you're adding flavor to on the grill. Keep the lid closed while smoking to get the most out of your Hickory Wood Chips.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1307,16 +1139,8 @@
           <t>67004</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/67004-67019-WhiskeyWoodChips-OnWhite-800px.png</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Whiskey barrel oak wood chips deliver a mild smoke flavor with a beautiful whiskey aroma. Whiskey barrel oak smoking chips as a whole are sweet and strong without being overpowering, ideal for bringing out the flavor of beef, pork, poultry, fish, fruit, and vegetables. Ideal for use in the Napoleon Smoker Pipe or Smoker Box accessories, or the integrated smoker tubes in the PRO665/825.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1337,16 +1161,8 @@
           <t>67005</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/cherry-wood-chips-bag-transparent-800px.png</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Cherry is a hardwood that is found all over the world. It has many different varieties with different properties. It has been bred for beauty, or to bear stone fruit like cherries. The smoke from Cherry Wood Chips is tart and fruity. It is best when used for smoking red meats like venison and beef. It is fantastic with pork, and even poultry. It is great for smoking fruits and vegetables too. To use your Cherry Wood Chips, soak them in water, or apple juice, ale, wine, cider, chardonnay, pinot noir, or even pineapple juice for added flavor. Remove them from the soaking liquid and load them into a Napoleon Smoker Pipe. Place the Smoker Pipe onto the sear plates of your grill to warm and begin to smoke. Or you can throw the Cherry Wood Chips right on the charcoal in an Apollo® 3 in 1 Charcoal Grill and Water Smoker, or directly into the integrated smoker tray on the Napoleon Prestige PRO™ Series PRO665RSIB Gas Grill. Once the chips begin to smoke, place your food onto the grill and close the lid or doors. To get the most flavor with your Cherry Wood Chips, remember to keep the lid closed while smoking to keep the smoke in.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1367,16 +1183,8 @@
           <t>67006</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/67006-67021-BrandyWoodChips-OnWhite-800px.png</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Brandy barrel oak wood chunks deliver a mild oak smoke with a sweet wine finish. They are the perfect complement to beef, pork, poultry, fish, fruit, and vegetables. Ideal for use in the Napoleon Smoker Pipe or Smoker Box accessories, or the integrated smoker tubes in the PRO665/825.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1397,16 +1205,8 @@
           <t>67007</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/apple-wood-chips-bag-transparent-800px.png</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Apple trees are a semi-hardwood that is found throughout most of the world's temperate climates. Apple Wood Chips are prized in the culinary world for their pleasant scent and the sweet smoke that comes with smoking using them. The flavor from smoking with Apple Wood Chips is very mild, another benefit to using these chips in smoking. The foods that benefit most from Apple Wood smoke are seafood, fish, and shellfish that benefit from the sweet treatment, like salmon. It is also fantastic with pork chops, tenderloin, and even veal. Apple Wood Chips are great for smoking fruits and vegetables too. When using Apple Wood Chips, soak them for at least 30 minutes in water, apple juice, ale, wine or cider, chardonnay, pinot noir or even pineapple juice. Remove the Apple Wood Chips from the soaking liquid and place them into the Napoleon Smoker Pipe, then place the pipe onto the sear plates of a gas grill. Conversely, you could place the soaked Apple Wood Chips into the smoker tray, integrated directly into the Napoleon Prestige PRO Series PRO665RSIB Gas Grill, or right onto the lit coals of an Apollo® 3 in 1 Charcoal Grill and Water Smoker. When the chips begin smoking, place your food directly on the grill and close the lid, trapping the sweet smoke in with the food. Remember to keep the lid closed and only check the food when necessary to get the most out of the Apple Wood Chip smoke flavor.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1449,11 +1249,7 @@
           <t>P500RSIBNK-3 NG</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Prestige-500-RSIB-Prod-Str-K-Knbs-On-800px.png</t>
-        </is>
-      </c>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
     </row>
     <row r="38">
@@ -1475,11 +1271,7 @@
           <t>P500RSIBNSS-3 NG</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Prestige-500-RSIB-Prod-Str-SS-Knbs-On-800px.png</t>
-        </is>
-      </c>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
     </row>
     <row r="39">
@@ -1501,11 +1293,7 @@
           <t>P665NSS NG</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Prestige-665-Prod-Str-SS-NoRotis-Knbs-On-800px.png</t>
-        </is>
-      </c>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
     </row>
     <row r="40">
@@ -1527,11 +1315,7 @@
           <t>P665RSIBNSS NG</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Prestige-665-RSIB-Prod-Str-SS-KnbsOn-800px.png</t>
-        </is>
-      </c>
+      <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
     </row>
     <row r="41">
@@ -1553,11 +1337,7 @@
           <t>PRO500RSIBNSS-3 NG</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/PrestigePRO-500-RSIB-Prod-Str-Knbs-On-800px.png</t>
-        </is>
-      </c>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
     </row>
     <row r="42">
@@ -1601,11 +1381,7 @@
           <t>RXT425SIBNK-1</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Rogue-RXT425SIB-1-Prod-Str-K-800px.png</t>
-        </is>
-      </c>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
     </row>
     <row r="44">
@@ -1627,11 +1403,7 @@
           <t>P500RSIBNMK-3-PHM</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Prestige-Phantom-P500RSIBPMK-3-PHM-Prod-Str-KnobsOn-wRotisserie-800px.png</t>
-        </is>
-      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
     </row>
     <row r="45">
@@ -1653,11 +1425,7 @@
           <t>RSE425RSIBNMK-1-PHM</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/RSE425SIBMK-1PHM-Prod-Closed_Str-800px.png</t>
-        </is>
-      </c>
+      <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
@@ -1833,16 +1601,8 @@
           <t>GPFTS-WNDSCRN</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/GPFS-wind-screen-square-transparent-800px.png</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Enjoying the great outdoors doesn't have to stop just because it's a little windy. Add the Square Windscreen to your St. Tropez or Kensington Patioflame® Table and keep the fun going even if there's a breeze. The five-inch tall tempered glass offers protection so that the flames don't get blown out.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1863,16 +1623,8 @@
           <t>GPFSE-WNDSCRN</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/GPFS-wind-screen-square-transparent-800px.png</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Enjoying the great outdoors doesn't have to stop just because it's a little windy. Add the Square Windscreen to your Hamptons Patioflame® Table and keep the fun going even if there's a breeze. The five inch tall tempered glass offers protection so that the flames don't get blown out.&lt;/p&gt;</t>
-        </is>
-      </c>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1893,11 +1645,7 @@
           <t>HAMP1-GY</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Hampton-Rect-Prod-Str-GY-flame-Shadow-800px.png</t>
-        </is>
-      </c>
+      <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
     </row>
     <row r="56">
@@ -1919,11 +1667,7 @@
           <t>HAMP2-GY</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Hampton-Sq-Prod-Str-GY-flame-shadow-800px.png</t>
-        </is>
-      </c>
+      <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
     </row>
     <row r="57">
@@ -1945,11 +1689,7 @@
           <t>KENS1-BZ-1</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Patioflame-Kensington-Rectangle-Prod-Str-LidOff-Shadow-800px.png</t>
-        </is>
-      </c>
+      <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
     </row>
     <row r="58">
@@ -1971,11 +1711,7 @@
           <t>KENS2-BZ-1</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Kensington-square-straight-800px.png</t>
-        </is>
-      </c>
+      <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
     </row>
     <row r="59">
@@ -1997,11 +1733,7 @@
           <t>KENS3-BZ</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Patioflame-Kensington-Round-Prod-Str-Shadow-800px.png</t>
-        </is>
-      </c>
+      <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr"/>
     </row>
     <row r="60">
@@ -2023,11 +1755,7 @@
           <t>STTR2-BZ</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/StTropez-Square-Prod-Str-LidOff-Flames-800px.png</t>
-        </is>
-      </c>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
     </row>
     <row r="61">
@@ -2049,11 +1777,7 @@
           <t>STTR1-BZ</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/StTropez-Rctngl-Prod-Str-LongEnd-LidOff-Flame-800px.png</t>
-        </is>
-      </c>
+      <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
     </row>
     <row r="62">
@@ -2075,11 +1799,7 @@
           <t>GPFCCN36</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/GPFCCN36-Nexus-Patioflame-Prod-800.png</t>
-        </is>
-      </c>
+      <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
     </row>
     <row r="63">
@@ -2123,11 +1843,7 @@
           <t>P500RSIBPSS-3 LP</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Prestige-500-RSIB-Prod-Str-SS-Knbs-On-800px.png</t>
-        </is>
-      </c>
+      <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
     </row>
     <row r="65">
@@ -2171,11 +1887,7 @@
           <t>P665RSIBPSS LP</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Prestige-665-RSIB-Prod-Str-SS-KnbsOn-800px.png</t>
-        </is>
-      </c>
+      <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
     </row>
     <row r="67">
@@ -2197,11 +1909,7 @@
           <t>PRO665RSIBPSS-3 LP</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Prestige-PRO665-3-RSIB-Prod-Str-Knbs-On-800px.png</t>
-        </is>
-      </c>
+      <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
     </row>
     <row r="68">
@@ -2223,11 +1931,7 @@
           <t>PRO500RSIBPSS-3 LP</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/PrestigePRO-500-RSIB-Prod-Str-Knbs-On-800px.png</t>
-        </is>
-      </c>
+      <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
     </row>
     <row r="69">
@@ -2249,11 +1953,7 @@
           <t>RXT425SIBPK-1</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Rogue-RXT425SIB-1-Prod-Str-K-800px.png</t>
-        </is>
-      </c>
+      <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
     </row>
     <row r="70">
@@ -2275,11 +1975,7 @@
           <t>RXT425SIBPSS-1</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Rogue-RXT425SIB-1-Prod-Str-SS-800px.png</t>
-        </is>
-      </c>
+      <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr"/>
     </row>
     <row r="71">
@@ -2301,11 +1997,7 @@
           <t>P500RSIBPMK-3-PHM</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/Prestige-Phantom-P500RSIBPMK-3-PHM-Prod-Str-KnobsOn-wRotisserie-800px.png</t>
-        </is>
-      </c>
+      <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
     </row>
     <row r="72">
@@ -2327,11 +2019,7 @@
           <t>RSE425RSIBPMK-1-PHM</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>/sites/default/files/products/RSE425SIBMK-1PHM-Prod-Closed_Str-800px.png</t>
-        </is>
-      </c>
+      <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>